<commit_message>
update database design and all value
</commit_message>
<xml_diff>
--- a/Documents/AllValues.xlsx
+++ b/Documents/AllValues.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="130">
   <si>
     <t>No.</t>
   </si>
@@ -66,21 +66,6 @@
     <t xml:space="preserve">Duration of meeting </t>
   </si>
   <si>
-    <t>greater than 0 ; required</t>
-  </si>
-  <si>
-    <t>mDurationMinute</t>
-  </si>
-  <si>
-    <t>greater than 0 and less than 60</t>
-  </si>
-  <si>
-    <t>mDurationHour</t>
-  </si>
-  <si>
-    <t>greater than 0 and less than 24</t>
-  </si>
-  <si>
     <t>mLocation</t>
   </si>
   <si>
@@ -103,15 +88,6 @@
   </si>
   <si>
     <t>Time to end searching</t>
-  </si>
-  <si>
-    <t>mExpiration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of day(s) for searching </t>
-  </si>
-  <si>
-    <t>Auto convert from week, month, year to day</t>
   </si>
   <si>
     <t>mBreakfast</t>
@@ -408,15 +384,6 @@
     <t>show = true; hide = false.</t>
   </si>
   <si>
-    <t>wType</t>
-  </si>
-  <si>
-    <t>Type to draw calendar</t>
-  </si>
-  <si>
-    <t>If type = list or day, do not need wEvent</t>
-  </si>
-  <si>
     <t>wEvent</t>
   </si>
   <si>
@@ -430,6 +397,24 @@
   </si>
   <si>
     <t>8-16 characters</t>
+  </si>
+  <si>
+    <t>mDuration minute(s)</t>
+  </si>
+  <si>
+    <t>mFromDay</t>
+  </si>
+  <si>
+    <t>mToDay</t>
+  </si>
+  <si>
+    <t>Day to start searching</t>
+  </si>
+  <si>
+    <t>format: ddmmyy</t>
+  </si>
+  <si>
+    <t>Day to end searching</t>
   </si>
 </sst>
 </file>
@@ -589,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -629,6 +614,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -955,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G55"/>
+  <dimension ref="B2:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,14 +962,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="B2" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
@@ -1007,13 +995,13 @@
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="20" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="21" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1033,7 +1021,7 @@
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="16"/>
+      <c r="G5" s="17"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
@@ -1045,33 +1033,35 @@
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="16"/>
+      <c r="F6" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="17"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="16"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
@@ -1079,737 +1069,719 @@
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="F8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="16"/>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="16"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="1">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="16"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="16"/>
+        <v>24</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+        <v>34</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
-        <v>14</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="26" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
-        <v>15</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="25" t="s">
-        <v>44</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="17"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>47</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="16"/>
+        <v>42</v>
+      </c>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="16"/>
+        <v>38</v>
+      </c>
+      <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="16"/>
+        <v>44</v>
+      </c>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="16"/>
       <c r="F21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="16"/>
+        <v>47</v>
+      </c>
+      <c r="G21" s="17"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>54</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E22" s="17"/>
       <c r="F22" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="16"/>
+        <v>49</v>
+      </c>
+      <c r="G22" s="17"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
-        <v>20</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="16"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="17"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>59</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E24" s="17"/>
       <c r="F24" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G24" s="16"/>
+        <v>54</v>
+      </c>
+      <c r="G24" s="17"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="16"/>
+        <v>38</v>
+      </c>
+      <c r="E25" s="17"/>
       <c r="F25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
-        <v>23</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G26" s="16"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
+        <v>26</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F28" s="4"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
+        <v>27</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="1">
-        <v>25</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="D29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="F29" s="4"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
+        <v>28</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="1">
-        <v>26</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="1">
-        <v>27</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="16"/>
+      <c r="G30" s="17"/>
     </row>
     <row r="31" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="1">
+        <v>30</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F32" s="4"/>
+      <c r="G32" s="17"/>
+    </row>
+    <row r="33" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1">
+        <v>31</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B32" s="1">
-        <v>29</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="G33" s="17"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="1">
+        <v>32</v>
+      </c>
+      <c r="C34" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="G32" s="16"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="1">
-        <v>30</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="16"/>
-    </row>
-    <row r="34" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B34" s="1">
-        <v>31</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G34" s="16"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
-        <v>32</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="24" t="s">
-        <v>93</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" s="17"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G36" s="16"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="38" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G38" s="16"/>
+        <v>97</v>
+      </c>
+      <c r="G38" s="17"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G39" s="16"/>
+        <v>99</v>
+      </c>
+      <c r="G39" s="17"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G40" s="16"/>
+        <v>123</v>
+      </c>
+      <c r="G40" s="17"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
+        <v>39</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="E41" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="G41" s="16"/>
+        <v>103</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="17"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="16"/>
+        <v>106</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" s="17"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="1">
-        <v>40</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G43" s="16"/>
+        <v>41</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="23" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="1">
-        <v>41</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="17"/>
+    </row>
+    <row r="45" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B45" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F45" s="6"/>
-      <c r="G45" s="16"/>
+        <v>96</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G45" s="17"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G46" s="16"/>
+        <v>113</v>
+      </c>
+      <c r="G46" s="17"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" s="1">
-        <v>44</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G47" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="22" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" s="1">
-        <v>45</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="21" t="s">
-        <v>123</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G48" s="17"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" s="1">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G49" s="16"/>
+        <v>120</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="17"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="1">
-        <v>47</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G50" s="16"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="1">
-        <v>48</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="F51" s="7"/>
-      <c r="G51" s="16"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" s="8"/>
@@ -1827,40 +1799,23 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="8"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="8"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C47:F47"/>
     <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:G17"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="G44:G47"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="G35:G43"/>
-    <mergeCell ref="G18:G34"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="G4:G16"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="G43:G46"/>
+    <mergeCell ref="F12:F16"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="G34:G42"/>
+    <mergeCell ref="G17:G33"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E23:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>